<commit_message>
SSLAS-123: Added Line2 to ScriptDoc.txt and added step to TestScript.xlsx
</commit_message>
<xml_diff>
--- a/TestScript.xlsx
+++ b/TestScript.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Keyword</t>
   </si>
@@ -46,6 +46,24 @@
   </si>
   <si>
     <t>Non-Proving</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Login_Username</t>
+  </si>
+  <si>
+    <t>ClinicUserDataRole</t>
+  </si>
+  <si>
+    <t>KeyInData</t>
+  </si>
+  <si>
+    <t>TestData</t>
+  </si>
+  <si>
+    <t>Step-002</t>
   </si>
 </sst>
 </file>
@@ -122,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -132,6 +150,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -434,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,6 +498,29 @@
         <v>8</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>